<commit_message>
fixed bugs #1, #3, #4, #5, #6, #7
</commit_message>
<xml_diff>
--- a/.bugs.xlsx
+++ b/.bugs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\apps\tlm_react_native\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B621A22-9175-45FE-AE8B-FAF9EF488537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EB22B0-E57E-4745-B814-A3883835A999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-900" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Device</t>
   </si>
@@ -77,6 +77,39 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>Alla creazione della notifica avviene un crash</t>
+  </si>
+  <si>
+    <t>Galaxy S22</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Fede, Mauro</t>
+  </si>
+  <si>
+    <t>Lembo</t>
+  </si>
+  <si>
+    <t>Elena</t>
+  </si>
+  <si>
+    <t>With Android &gt; 13, it is necessary to add the permissions &lt;uses-permission android:name="android.permission.USE_EXACT_ALARM" /&gt;</t>
+  </si>
+  <si>
+    <t>With Android &gt; 13, it's not possible anymore to use READ_EXTERNAL_STORAGE, but READ_MEDIA_IMAGES and other two permissions must be used</t>
+  </si>
+  <si>
+    <t>Android &gt; 13</t>
+  </si>
+  <si>
+    <t>Can't reproduce</t>
+  </si>
+  <si>
+    <t>Should be the same as bug #5</t>
   </si>
 </sst>
 </file>
@@ -138,7 +171,10 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -223,14 +259,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BF78EB4-1204-494F-A981-4762F6205C8D}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E7" xr:uid="{5BF78EB4-1204-494F-A981-4762F6205C8D}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A6E1745A-F0E6-4902-A4FA-7DF47C13BCD4}" name="ID" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{E7E227B8-7E33-436D-A7C6-312190FBF650}" name="Bug" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{41334200-9BD3-4768-AED4-8DBCE25B46A5}" name="Device" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{0DB75320-01E3-46C6-8F6D-26FB55202B6B}" name="Notes" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{82EDAA82-FEE6-4265-B357-73562C1609A2}" name="Status" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BF78EB4-1204-494F-A981-4762F6205C8D}" name="Table1" displayName="Table1" ref="A1:F8" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F8" xr:uid="{5BF78EB4-1204-494F-A981-4762F6205C8D}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{A6E1745A-F0E6-4902-A4FA-7DF47C13BCD4}" name="ID" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{E7E227B8-7E33-436D-A7C6-312190FBF650}" name="Bug" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{41334200-9BD3-4768-AED4-8DBCE25B46A5}" name="Device" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{65C65464-45CF-44E3-84CF-FB53A0E4BF57}" name="User" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{0DB75320-01E3-46C6-8F6D-26FB55202B6B}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{82EDAA82-FEE6-4265-B357-73562C1609A2}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -499,21 +536,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E408"/>
+  <dimension ref="A1:F408"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F7" sqref="A7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="62.42578125" customWidth="1"/>
-    <col min="3" max="4" width="54.7109375" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" customWidth="1"/>
+    <col min="5" max="5" width="54.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -524,24 +563,34 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -552,56 +601,111 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -996,7 +1100,7 @@
     <row r="408" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{B9F87A35-6B03-4B6F-B340-3BEB044D929C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{B9F87A35-6B03-4B6F-B340-3BEB044D929C}">
       <formula1>"OK,KO,WIP,ON HOLD"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>